<commit_message>
Add 2021 VMMCcov assuming 2017-2030 scale-up
</commit_message>
<xml_diff>
--- a/Config/Circumcision_parameters_04092020.xlsx
+++ b/Config/Circumcision_parameters_04092020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6D54FB-71BF-4119-B263-57179906C19D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8172204D-F1E9-4AA2-A6E1-2C7AFEB0467A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="521" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -187,10 +187,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2924,26 +2924,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4">
         <v>1960</v>
@@ -2967,16 +2967,19 @@
         <v>2020</v>
       </c>
       <c r="I2" s="8">
+        <v>2021</v>
+      </c>
+      <c r="J2" s="8">
         <v>2030</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -3002,22 +3005,26 @@
         <f>((0.702*0.626)*2)-G4</f>
         <v>0.45890399999999992</v>
       </c>
-      <c r="H3" s="11">
-        <f>G3+(H$2-G$2)*J3</f>
+      <c r="H3" s="10">
+        <f>G3+(H$2-G$2)*K3</f>
         <v>0.51454153846153838</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="10">
+        <f>G3+(I$2-G$2)*K3</f>
+        <v>0.53308738461538452</v>
+      </c>
+      <c r="J3" s="9">
         <v>0.7</v>
       </c>
-      <c r="J3" s="9">
-        <f>(I3-G3)/((I$2-1)-(G$2-1))</f>
+      <c r="K3" s="9">
+        <f>(J3-G3)/((J$2-1)-(G$2-1))</f>
         <v>1.8545846153846156E-2</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -3042,25 +3049,29 @@
       <c r="G4" s="6">
         <v>0.42</v>
       </c>
-      <c r="H4" s="11">
-        <f t="shared" ref="H4:H6" si="0">G4+(H$2-G$2)*J4</f>
+      <c r="H4" s="10">
+        <f t="shared" ref="H4:H6" si="0">G4+(H$2-G$2)*K4</f>
         <v>0.48461538461538461</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="10">
+        <f t="shared" ref="I4:I6" si="1">G4+(I$2-G$2)*K4</f>
+        <v>0.50615384615384618</v>
+      </c>
+      <c r="J4" s="9">
         <v>0.7</v>
       </c>
-      <c r="J4" s="9">
-        <f>(I4-G4)/((I$2-1)-(G$2-1))</f>
+      <c r="K4" s="9">
+        <f>(J4-G4)/((J$2-1)-(G$2-1))</f>
         <v>2.1538461538461538E-2</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>16</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -3079,22 +3090,26 @@
         <f>0.618*0.515</f>
         <v>0.31827</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <f t="shared" si="0"/>
         <v>0.40636153846153844</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="10">
+        <f t="shared" si="1"/>
+        <v>0.43572538461538457</v>
+      </c>
+      <c r="J5" s="9">
         <v>0.7</v>
       </c>
-      <c r="J5" s="9">
-        <f>(I5-G5)/((I$2-1)-(G$2-1))</f>
+      <c r="K5" s="9">
+        <f>(J5-G5)/((J$2-1)-(G$2-1))</f>
         <v>2.936384615384615E-2</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -3113,57 +3128,61 @@
         <f>0.54*0.378</f>
         <v>0.20412000000000002</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f t="shared" si="0"/>
         <v>0.31855384615384619</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="10">
+        <f t="shared" si="1"/>
+        <v>0.35669846153846152</v>
+      </c>
+      <c r="J6" s="9">
         <v>0.7</v>
       </c>
-      <c r="J6" s="9">
-        <f>(I6-G6)/((I$2-1)-(G$2-1))</f>
+      <c r="K6" s="9">
+        <f>(J6-G6)/((J$2-1)-(G$2-1))</f>
         <v>3.8144615384615381E-2</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I7" s="10" t="s">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="K8" t="s">
+      <c r="J8" s="11"/>
+      <c r="L8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2016</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="J9" s="11"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10">
         <v>0.41199999999999998</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="K10" t="s">
+      <c r="J10" s="11"/>
+      <c r="L10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -3171,12 +3190,12 @@
         <v>0.35799999999999998</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="I11" s="10"/>
-      <c r="K11" t="s">
+      <c r="J11" s="11"/>
+      <c r="L11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -3184,12 +3203,12 @@
         <v>0.34399999999999997</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="I12" s="10"/>
-      <c r="K12" t="s">
+      <c r="J12" s="11"/>
+      <c r="L12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -3197,20 +3216,20 @@
         <v>0.215</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14">
         <v>0.20499999999999999</v>
       </c>
-      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I7:I12"/>
+    <mergeCell ref="J7:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>